<commit_message>
update patient with random data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/requestBodyDetails.xlsx
+++ b/src/test/resources/testData/requestBodyDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\eclipse-workspace\T7_RestlessCoders_DieticianAPI_Hackathon_nov_2023\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77135114-1D97-4923-B4DB-CEFB5D943ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5BDFE9-6ED1-404D-88F8-E91C5513C80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0E5AE6ED-B2BD-49D4-8895-9B2C6FFBF544}"/>
   </bookViews>
@@ -75,12 +75,6 @@
     <t>patientId</t>
   </si>
   <si>
-    <t>test23</t>
-  </si>
-  <si>
-    <t>test24</t>
-  </si>
-  <si>
     <t>test23@gmail.com</t>
   </si>
   <si>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>1991-01-24</t>
+  </si>
+  <si>
+    <t>test25</t>
+  </si>
+  <si>
+    <t>test26</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,16 +497,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1111111123</v>
+        <v>1111111125</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -515,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>133</v>
@@ -523,16 +523,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1111111124</v>
+        <v>1111111126</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -541,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3">
         <v>133</v>

</xml_diff>